<commit_message>
Add updated code and output graphs for data analysis
</commit_message>
<xml_diff>
--- a/datasets/ProductA.xlsx
+++ b/datasets/ProductA.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitin\OneDrive\Documents\Infosys Springboard Internship Files\NitinMishra-Infosys-Nov24\datasets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6346DC7E-0E6F-498A-B5AC-5E04FB937CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="ProductA"/>
+    <sheet name="ProductA" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">ProductA!$A$1:$B$213</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -28,8 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -72,35 +77,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -111,10 +111,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -152,71 +152,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -244,7 +244,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -267,11 +267,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -280,13 +280,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -296,7 +296,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -305,7 +305,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -314,7 +314,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -322,10 +322,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -390,21 +390,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B213"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="A213" sqref="A213"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="10.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -412,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>44531</v>
       </c>
@@ -420,7 +422,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>44532</v>
       </c>
@@ -428,7 +430,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>44533</v>
       </c>
@@ -436,7 +438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>44534</v>
       </c>
@@ -444,7 +446,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>44535</v>
       </c>
@@ -452,7 +454,7 @@
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>44536</v>
       </c>
@@ -460,7 +462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>44537</v>
       </c>
@@ -468,7 +470,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>44538</v>
       </c>
@@ -476,7 +478,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>44539</v>
       </c>
@@ -484,7 +486,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>44540</v>
       </c>
@@ -492,7 +494,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>44541</v>
       </c>
@@ -500,7 +502,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>44542</v>
       </c>
@@ -508,7 +510,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>44543</v>
       </c>
@@ -516,7 +518,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44544</v>
       </c>
@@ -524,7 +526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>44545</v>
       </c>
@@ -532,7 +534,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>44546</v>
       </c>
@@ -540,7 +542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>44547</v>
       </c>
@@ -548,7 +550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>44548</v>
       </c>
@@ -556,7 +558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>44549</v>
       </c>
@@ -564,7 +566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>44550</v>
       </c>
@@ -572,7 +574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>44551</v>
       </c>
@@ -580,7 +582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>44552</v>
       </c>
@@ -588,7 +590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>44553</v>
       </c>
@@ -596,7 +598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>44554</v>
       </c>
@@ -604,7 +606,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>44555</v>
       </c>
@@ -612,7 +614,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>44556</v>
       </c>
@@ -620,7 +622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>44557</v>
       </c>
@@ -628,7 +630,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>44558</v>
       </c>
@@ -636,7 +638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>44559</v>
       </c>
@@ -644,7 +646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>44560</v>
       </c>
@@ -652,7 +654,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>44561</v>
       </c>
@@ -660,7 +662,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>44562</v>
       </c>
@@ -668,7 +670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>44563</v>
       </c>
@@ -676,7 +678,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>44564</v>
       </c>
@@ -684,7 +686,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>44565</v>
       </c>
@@ -692,7 +694,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>44566</v>
       </c>
@@ -700,7 +702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>44567</v>
       </c>
@@ -708,7 +710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>44568</v>
       </c>
@@ -716,7 +718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>44569</v>
       </c>
@@ -724,7 +726,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>44570</v>
       </c>
@@ -732,7 +734,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>44571</v>
       </c>
@@ -740,7 +742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>44572</v>
       </c>
@@ -748,7 +750,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>44573</v>
       </c>
@@ -756,7 +758,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44574</v>
       </c>
@@ -764,7 +766,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>44575</v>
       </c>
@@ -772,7 +774,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>44576</v>
       </c>
@@ -780,7 +782,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>44577</v>
       </c>
@@ -788,7 +790,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>44578</v>
       </c>
@@ -796,7 +798,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>44579</v>
       </c>
@@ -804,7 +806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>44580</v>
       </c>
@@ -812,7 +814,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>44581</v>
       </c>
@@ -820,7 +822,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>44582</v>
       </c>
@@ -828,7 +830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>44583</v>
       </c>
@@ -836,7 +838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>44584</v>
       </c>
@@ -844,7 +846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>44585</v>
       </c>
@@ -852,7 +854,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>44586</v>
       </c>
@@ -860,7 +862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>44587</v>
       </c>
@@ -868,7 +870,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>44588</v>
       </c>
@@ -876,7 +878,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>44589</v>
       </c>
@@ -884,7 +886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>44590</v>
       </c>
@@ -892,7 +894,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row r="62" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>44591</v>
       </c>
@@ -900,7 +902,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row r="63" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>44592</v>
       </c>
@@ -908,7 +910,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row r="64" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>44593</v>
       </c>
@@ -916,7 +918,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row r="65" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>44594</v>
       </c>
@@ -924,7 +926,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row r="66" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>44595</v>
       </c>
@@ -932,7 +934,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row r="67" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>44596</v>
       </c>
@@ -940,7 +942,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row r="68" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>44597</v>
       </c>
@@ -948,7 +950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row r="69" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>44598</v>
       </c>
@@ -956,7 +958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row r="70" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>44599</v>
       </c>
@@ -964,7 +966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row r="71" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>44600</v>
       </c>
@@ -972,7 +974,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row r="72" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>44601</v>
       </c>
@@ -980,7 +982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row r="73" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>44602</v>
       </c>
@@ -988,7 +990,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row r="74" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>44603</v>
       </c>
@@ -996,7 +998,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row r="75" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>44604</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row r="76" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>44605</v>
       </c>
@@ -1012,7 +1014,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row r="77" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>44606</v>
       </c>
@@ -1020,7 +1022,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row r="78" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>44607</v>
       </c>
@@ -1028,7 +1030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row r="79" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>44608</v>
       </c>
@@ -1036,7 +1038,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row r="80" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>44609</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row r="81" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>44610</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row r="82" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>44611</v>
       </c>
@@ -1060,7 +1062,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row r="83" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>44612</v>
       </c>
@@ -1068,7 +1070,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row r="84" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>44613</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row r="85" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>44614</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row r="86" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>44615</v>
       </c>
@@ -1092,7 +1094,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row r="87" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>44616</v>
       </c>
@@ -1100,7 +1102,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row r="88" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>44617</v>
       </c>
@@ -1108,7 +1110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row r="89" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>44618</v>
       </c>
@@ -1116,7 +1118,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row r="90" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>44619</v>
       </c>
@@ -1124,7 +1126,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row r="91" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>44620</v>
       </c>
@@ -1132,7 +1134,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row r="92" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>44621</v>
       </c>
@@ -1140,7 +1142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row r="93" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>44622</v>
       </c>
@@ -1148,7 +1150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row r="94" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>44623</v>
       </c>
@@ -1156,7 +1158,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row r="95" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>44624</v>
       </c>
@@ -1164,7 +1166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row r="96" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>44625</v>
       </c>
@@ -1172,7 +1174,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row r="97" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>44626</v>
       </c>
@@ -1180,7 +1182,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row r="98" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>44627</v>
       </c>
@@ -1188,7 +1190,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row r="99" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>44628</v>
       </c>
@@ -1196,7 +1198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+    <row r="100" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>44629</v>
       </c>
@@ -1204,7 +1206,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+    <row r="101" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>44630</v>
       </c>
@@ -1212,7 +1214,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+    <row r="102" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>44631</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+    <row r="103" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>44632</v>
       </c>
@@ -1228,7 +1230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+    <row r="104" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>44633</v>
       </c>
@@ -1236,7 +1238,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+    <row r="105" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>44634</v>
       </c>
@@ -1244,7 +1246,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+    <row r="106" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>44635</v>
       </c>
@@ -1252,7 +1254,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
+    <row r="107" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>44636</v>
       </c>
@@ -1260,7 +1262,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+    <row r="108" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>44637</v>
       </c>
@@ -1268,7 +1270,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
+    <row r="109" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>44638</v>
       </c>
@@ -1276,7 +1278,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+    <row r="110" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>44639</v>
       </c>
@@ -1284,7 +1286,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+    <row r="111" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>44640</v>
       </c>
@@ -1292,7 +1294,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
+    <row r="112" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>44641</v>
       </c>
@@ -1300,7 +1302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
+    <row r="113" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>44642</v>
       </c>
@@ -1308,7 +1310,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
+    <row r="114" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>44643</v>
       </c>
@@ -1316,7 +1318,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
+    <row r="115" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>44644</v>
       </c>
@@ -1324,7 +1326,7 @@
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
+    <row r="116" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>44645</v>
       </c>
@@ -1332,7 +1334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
+    <row r="117" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>44646</v>
       </c>
@@ -1340,7 +1342,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
+    <row r="118" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>44647</v>
       </c>
@@ -1348,7 +1350,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
+    <row r="119" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>44648</v>
       </c>
@@ -1356,7 +1358,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
+    <row r="120" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>44649</v>
       </c>
@@ -1364,7 +1366,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
+    <row r="121" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>44650</v>
       </c>
@@ -1372,7 +1374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
+    <row r="122" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>44651</v>
       </c>
@@ -1380,7 +1382,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
+    <row r="123" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>44652</v>
       </c>
@@ -1388,7 +1390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
+    <row r="124" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>44653</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
+    <row r="125" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>44654</v>
       </c>
@@ -1404,7 +1406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
+    <row r="126" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>44655</v>
       </c>
@@ -1412,7 +1414,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+    <row r="127" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>44656</v>
       </c>
@@ -1420,7 +1422,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+    <row r="128" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>44657</v>
       </c>
@@ -1428,7 +1430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
+    <row r="129" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>44658</v>
       </c>
@@ -1436,7 +1438,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
+    <row r="130" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>44659</v>
       </c>
@@ -1444,7 +1446,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
+    <row r="131" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>44660</v>
       </c>
@@ -1452,7 +1454,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
+    <row r="132" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>44661</v>
       </c>
@@ -1460,7 +1462,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
+    <row r="133" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>44662</v>
       </c>
@@ -1468,7 +1470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
+    <row r="134" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>44663</v>
       </c>
@@ -1476,7 +1478,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
+    <row r="135" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>44664</v>
       </c>
@@ -1484,7 +1486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
+    <row r="136" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>44665</v>
       </c>
@@ -1492,7 +1494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
+    <row r="137" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>44666</v>
       </c>
@@ -1500,7 +1502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
+    <row r="138" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>44667</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
+    <row r="139" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>44668</v>
       </c>
@@ -1516,7 +1518,7 @@
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
+    <row r="140" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>44669</v>
       </c>
@@ -1524,7 +1526,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
+    <row r="141" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>44670</v>
       </c>
@@ -1532,7 +1534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
+    <row r="142" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>44671</v>
       </c>
@@ -1540,7 +1542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
+    <row r="143" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>44672</v>
       </c>
@@ -1548,7 +1550,7 @@
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
+    <row r="144" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>44673</v>
       </c>
@@ -1556,7 +1558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
+    <row r="145" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
         <v>44674</v>
       </c>
@@ -1564,7 +1566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
+    <row r="146" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>44675</v>
       </c>
@@ -1572,7 +1574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
+    <row r="147" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>44676</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
+    <row r="148" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>44677</v>
       </c>
@@ -1588,7 +1590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
+    <row r="149" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>44678</v>
       </c>
@@ -1596,7 +1598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
+    <row r="150" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>44679</v>
       </c>
@@ -1604,7 +1606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
+    <row r="151" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
         <v>44680</v>
       </c>
@@ -1612,7 +1614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
+    <row r="152" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>44681</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
+    <row r="153" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>44682</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
+    <row r="154" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>44683</v>
       </c>
@@ -1636,7 +1638,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
+    <row r="155" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>44684</v>
       </c>
@@ -1644,7 +1646,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
+    <row r="156" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>44685</v>
       </c>
@@ -1652,7 +1654,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
+    <row r="157" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
         <v>44686</v>
       </c>
@@ -1660,7 +1662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
+    <row r="158" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>44687</v>
       </c>
@@ -1668,7 +1670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
+    <row r="159" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>44688</v>
       </c>
@@ -1676,7 +1678,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
+    <row r="160" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>44689</v>
       </c>
@@ -1684,7 +1686,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
+    <row r="161" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>44690</v>
       </c>
@@ -1692,7 +1694,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
+    <row r="162" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>44691</v>
       </c>
@@ -1700,7 +1702,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
+    <row r="163" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
         <v>44692</v>
       </c>
@@ -1708,7 +1710,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
+    <row r="164" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>44693</v>
       </c>
@@ -1716,7 +1718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
+    <row r="165" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>44694</v>
       </c>
@@ -1724,7 +1726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
+    <row r="166" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>44695</v>
       </c>
@@ -1732,7 +1734,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
+    <row r="167" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
         <v>44696</v>
       </c>
@@ -1740,7 +1742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
+    <row r="168" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
         <v>44697</v>
       </c>
@@ -1748,7 +1750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
+    <row r="169" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
         <v>44698</v>
       </c>
@@ -1756,7 +1758,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
+    <row r="170" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
         <v>44699</v>
       </c>
@@ -1764,7 +1766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
+    <row r="171" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
         <v>44700</v>
       </c>
@@ -1772,7 +1774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
+    <row r="172" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
         <v>44701</v>
       </c>
@@ -1780,7 +1782,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+    <row r="173" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
         <v>44702</v>
       </c>
@@ -1788,7 +1790,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
+    <row r="174" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
         <v>44703</v>
       </c>
@@ -1796,7 +1798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+    <row r="175" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
         <v>44704</v>
       </c>
@@ -1804,7 +1806,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
+    <row r="176" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
         <v>44705</v>
       </c>
@@ -1812,7 +1814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
+    <row r="177" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
         <v>44706</v>
       </c>
@@ -1820,7 +1822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
+    <row r="178" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
         <v>44707</v>
       </c>
@@ -1828,7 +1830,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
+    <row r="179" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
         <v>44708</v>
       </c>
@@ -1836,7 +1838,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
+    <row r="180" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
         <v>44709</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
+    <row r="181" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
         <v>44710</v>
       </c>
@@ -1852,7 +1854,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
+    <row r="182" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
         <v>44711</v>
       </c>
@@ -1860,7 +1862,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
+    <row r="183" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
         <v>44712</v>
       </c>
@@ -1868,7 +1870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
+    <row r="184" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
         <v>44713</v>
       </c>
@@ -1876,7 +1878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="185" customHeight="1" ht="18.75">
+    <row r="185" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
         <v>44714</v>
       </c>
@@ -1884,7 +1886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="186" customHeight="1" ht="18.75">
+    <row r="186" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
         <v>44715</v>
       </c>
@@ -1892,7 +1894,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="187" customHeight="1" ht="18.75">
+    <row r="187" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
         <v>44716</v>
       </c>
@@ -1900,7 +1902,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="188" customHeight="1" ht="18.75">
+    <row r="188" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
         <v>44717</v>
       </c>
@@ -1908,7 +1910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="189" customHeight="1" ht="18.75">
+    <row r="189" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
         <v>44718</v>
       </c>
@@ -1916,7 +1918,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="190" customHeight="1" ht="18.75">
+    <row r="190" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
         <v>44719</v>
       </c>
@@ -1924,7 +1926,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
+    <row r="191" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>44720</v>
       </c>
@@ -1932,7 +1934,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="18.75">
+    <row r="192" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>44721</v>
       </c>
@@ -1940,7 +1942,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
+    <row r="193" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>44722</v>
       </c>
@@ -1948,7 +1950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="18.75">
+    <row r="194" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
         <v>44723</v>
       </c>
@@ -1956,7 +1958,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="18.75">
+    <row r="195" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>44724</v>
       </c>
@@ -1964,7 +1966,7 @@
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
+    <row r="196" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>44725</v>
       </c>
@@ -1972,7 +1974,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="197" customHeight="1" ht="18.75">
+    <row r="197" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>44726</v>
       </c>
@@ -1980,7 +1982,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
+    <row r="198" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>44727</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
+    <row r="199" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>44728</v>
       </c>
@@ -1996,7 +1998,7 @@
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
+    <row r="200" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>44729</v>
       </c>
@@ -2004,7 +2006,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
+    <row r="201" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>44730</v>
       </c>
@@ -2012,7 +2014,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
+    <row r="202" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>44731</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="203" customHeight="1" ht="18.75">
+    <row r="203" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="3">
         <v>44732</v>
       </c>
@@ -2028,7 +2030,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="204" customHeight="1" ht="18.75">
+    <row r="204" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>44733</v>
       </c>
@@ -2036,7 +2038,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="205" customHeight="1" ht="18.75">
+    <row r="205" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>44734</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="206" customHeight="1" ht="18.75">
+    <row r="206" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>44735</v>
       </c>
@@ -2052,7 +2054,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75">
+    <row r="207" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>44736</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75">
+    <row r="208" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>44737</v>
       </c>
@@ -2068,7 +2070,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="18.75">
+    <row r="209" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>44738</v>
       </c>
@@ -2076,7 +2078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18.75">
+    <row r="210" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>44739</v>
       </c>
@@ -2084,7 +2086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="18.75">
+    <row r="211" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>44740</v>
       </c>
@@ -2092,7 +2094,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="18.75">
+    <row r="212" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="3">
         <v>44741</v>
       </c>
@@ -2100,7 +2102,7 @@
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="18.75">
+    <row r="213" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>44742</v>
       </c>

</xml_diff>